<commit_message>
New API methods added
</commit_message>
<xml_diff>
--- a/src/main/resources/COM_OrderCreation_Testdata.xlsx
+++ b/src/main/resources/COM_OrderCreation_Testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATION\uiregression-suite\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AUTOMATION\OMSAutomation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -131,43 +131,43 @@
     <t>rafaelarmandonietoparra@gmail.com</t>
   </si>
   <si>
+    <t>correo@pruebas11.cl</t>
+  </si>
+  <si>
+    <t>Sole</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
+  </si>
+  <si>
+    <t>FCVChile</t>
+  </si>
+  <si>
+    <t>Pay Using MercadoPago</t>
+  </si>
+  <si>
+    <t>Credit Card</t>
+  </si>
+  <si>
+    <t>CreditcardNumber</t>
+  </si>
+  <si>
+    <t>ExpirationDate</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>RUT</t>
+  </si>
+  <si>
+    <t>1.111.111-11</t>
+  </si>
+  <si>
+    <t>TC05</t>
+  </si>
+  <si>
     <t>TC03</t>
-  </si>
-  <si>
-    <t>correo@pruebas11.cl</t>
-  </si>
-  <si>
-    <t>Sole</t>
-  </si>
-  <si>
-    <t>Pruebas</t>
-  </si>
-  <si>
-    <t>FCVChile</t>
-  </si>
-  <si>
-    <t>Pay Using MercadoPago</t>
-  </si>
-  <si>
-    <t>Credit Card</t>
-  </si>
-  <si>
-    <t>TC04</t>
-  </si>
-  <si>
-    <t>CreditcardNumber</t>
-  </si>
-  <si>
-    <t>ExpirationDate</t>
-  </si>
-  <si>
-    <t>CVV</t>
-  </si>
-  <si>
-    <t>RUT</t>
-  </si>
-  <si>
-    <t>1.111.111-11</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,36 +593,36 @@
         <v>22</v>
       </c>
       <c r="W1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" t="s">
         <v>43</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>44</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -640,10 +640,10 @@
         <v>32</v>
       </c>
       <c r="T2" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" t="s">
         <v>40</v>
-      </c>
-      <c r="U2" t="s">
-        <v>41</v>
       </c>
       <c r="W2">
         <v>371180303257522</v>
@@ -655,27 +655,27 @@
         <v>1234</v>
       </c>
       <c r="Z2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -699,10 +699,10 @@
         <v>32</v>
       </c>
       <c r="T3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" t="s">
         <v>40</v>
-      </c>
-      <c r="U3" t="s">
-        <v>41</v>
       </c>
       <c r="W3">
         <v>371180303257522</v>
@@ -714,12 +714,12 @@
         <v>1234</v>
       </c>
       <c r="Z3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>

</xml_diff>